<commit_message>
nueva implementacion de scripts.
</commit_message>
<xml_diff>
--- a/excel/ActionScripts.xlsx
+++ b/excel/ActionScripts.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Parameters" sheetId="2" r:id="rId2"/>
-    <sheet name="Objects" sheetId="3" r:id="rId3"/>
+    <sheet name="LoginDavid" sheetId="4" r:id="rId2"/>
+    <sheet name="Parameters" sheetId="2" r:id="rId3"/>
+    <sheet name="Objects" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Step</t>
   </si>
@@ -43,9 +44,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>compto</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -73,9 +71,6 @@
     <t>Maria$52</t>
   </si>
   <si>
-    <t>new project</t>
-  </si>
-  <si>
     <t>Locator</t>
   </si>
   <si>
@@ -103,9 +98,6 @@
     <t>//button[@class='mat-raised-button']</t>
   </si>
   <si>
-    <t>//a[contains(text(),'new project')]</t>
-  </si>
-  <si>
     <t>Destination Locator</t>
   </si>
   <si>
@@ -115,9 +107,6 @@
     <t>Screenshot</t>
   </si>
   <si>
-    <t>Verify if the page "Create a new project" is displayed.</t>
-  </si>
-  <si>
     <t>Click on "Getting Started"</t>
   </si>
   <si>
@@ -128,6 +117,12 @@
   </si>
   <si>
     <t>Value locator</t>
+  </si>
+  <si>
+    <t>davidpena</t>
+  </si>
+  <si>
+    <t>Hexaware123</t>
   </si>
 </sst>
 </file>
@@ -480,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,25 +500,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -534,10 +529,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -548,13 +543,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -568,13 +563,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -588,16 +583,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -611,16 +606,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -634,40 +629,21 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
+      <c r="C8" s="3"/>
+      <c r="F8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -680,6 +656,177 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
+      <c r="F8" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -690,10 +837,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -701,11 +848,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -713,16 +860,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>